<commit_message>
feat: finish Sell function
</commit_message>
<xml_diff>
--- a/THONG_TIN.xlsx
+++ b/THONG_TIN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\testProject\auto-complete-docx-form\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD83847-A626-4AE6-A882-941C37B35DFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35AB9775-B243-4BCE-886F-89A6662BA67B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -642,27 +642,27 @@
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5546875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="30.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.44140625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="27.88671875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="44.21875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15" style="5" customWidth="1"/>
-    <col min="10" max="10" width="14" style="1" customWidth="1"/>
-    <col min="11" max="11" width="21" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="11.77734375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="18.5546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="43.21875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" style="5" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="16.109375" style="1" customWidth="1"/>
     <col min="12" max="12" width="12.44140625" style="1" customWidth="1"/>
     <col min="13" max="13" width="26.33203125" style="1" customWidth="1"/>
     <col min="14" max="14" width="21.6640625" style="5" customWidth="1"/>
     <col min="15" max="15" width="18.21875" style="5" customWidth="1"/>
-    <col min="16" max="16" width="11.77734375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.6640625" style="1" customWidth="1"/>
     <col min="17" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>

</xml_diff>